<commit_message>
Respaldo proyecto Pagos GyG
</commit_message>
<xml_diff>
--- a/4.2. GyG Resúmenes - Control resúmenes.xlsx
+++ b/4.2. GyG Resúmenes - Control resúmenes.xlsx
@@ -669,11 +669,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A131" sqref="A131"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6037,7 +6037,48 @@
       </c>
       <c r="I131" s="63" t="inlineStr"/>
     </row>
-    <row r="132"/>
+    <row r="132">
+      <c r="A132" s="59" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" s="60" t="n"/>
+      <c r="C132" s="61" t="inlineStr">
+        <is>
+          <t>Familia Navarro Assing</t>
+        </is>
+      </c>
+      <c r="D132" s="61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NaN</t>
+        </is>
+      </c>
+      <c r="E132" s="61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Calle Güigüe Nro. 88-54</t>
+        </is>
+      </c>
+      <c r="F132" s="62" t="inlineStr">
+        <is>
+          <t>enero/2017</t>
+        </is>
+      </c>
+      <c r="G132" s="62" t="inlineStr">
+        <is>
+          <t>junio/2020</t>
+        </is>
+      </c>
+      <c r="H132" s="62" t="inlineStr">
+        <is>
+          <t>19/06/2020 08:53 pm</t>
+        </is>
+      </c>
+      <c r="I132" s="63" t="inlineStr">
+        <is>
+          <t>Saldos</t>
+        </is>
+      </c>
+    </row>
+    <row r="133"/>
   </sheetData>
   <autoFilter ref="A1:H1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>